<commit_message>
Saving the corresponding LibreOffice file as an Excel file in 1-ipip-50_item_sample/ipip-50_item_sample-i_am.xlsx .
</commit_message>
<xml_diff>
--- a/questionnaires/1-ipip-50_item_sample/ipip-50_item_sample-i_am.xlsx
+++ b/questionnaires/1-ipip-50_item_sample/ipip-50_item_sample-i_am.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="IPIP Big 5 Sample Questionnaire" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Score Values for .csv" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="83">
   <si>
     <t xml:space="preserve">IPIP 50 Item Big Five Sample Questionnaire</t>
   </si>
@@ -290,6 +291,9 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use right-click → Paste Special → Paste Special… to paste just the score here, then use File → Save As… to save that as a .csv file</t>
   </si>
 </sst>
 </file>
@@ -2651,7 +2655,7 @@
         <v>-10</v>
       </c>
       <c r="D64" s="15" t="str">
-        <f aca="false">IF(C64&lt;=20,"Very Low",IF(C64&lt;=40,"Low",IF(C64&lt;60,"Average",IF(C64&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(C64&lt;=20,"Very Low",IF(C64&lt;=36,"Low",IF(C64&lt;=46,"A Little Low",IF(C64&lt;=53,"Average",IF(C64&lt;=63,"A Little High",IF(C64&lt;=80,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -2668,7 +2672,7 @@
         <v>-10</v>
       </c>
       <c r="D65" s="15" t="str">
-        <f aca="false">IF(C65&lt;=20,"Very Low",IF(C65&lt;=40,"Low",IF(C65&lt;60,"Average",IF(C65&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(C65&lt;=20,"Very Low",IF(C65&lt;=36,"Low",IF(C65&lt;=46,"A Little Low",IF(C65&lt;=53,"Average",IF(C65&lt;=63,"A Little High",IF(C65&lt;=80,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -2685,7 +2689,7 @@
         <v>-10</v>
       </c>
       <c r="D66" s="15" t="str">
-        <f aca="false">IF(C66&lt;=20,"Very Low",IF(C66&lt;=40,"Low",IF(C66&lt;60,"Average",IF(C66&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(C66&lt;=20,"Very Low",IF(C66&lt;=36,"Low",IF(C66&lt;=46,"A Little Low",IF(C66&lt;=53,"Average",IF(C66&lt;=63,"A Little High",IF(C66&lt;=80,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -2702,7 +2706,7 @@
         <v>-10</v>
       </c>
       <c r="D67" s="15" t="str">
-        <f aca="false">IF(C67&lt;=20,"Very Low",IF(C67&lt;=40,"Low",IF(C67&lt;60,"Average",IF(C67&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(C67&lt;=20,"Very Low",IF(C67&lt;=36,"Low",IF(C67&lt;=46,"A Little Low",IF(C67&lt;=53,"Average",IF(C67&lt;=63,"A Little High",IF(C67&lt;=80,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -2719,7 +2723,7 @@
         <v>-10</v>
       </c>
       <c r="D68" s="15" t="str">
-        <f aca="false">IF(C68&lt;=20,"Very Low",IF(C68&lt;=40,"Low",IF(C68&lt;60,"Average",IF(C68&lt;80,"High","Very High"))))</f>
+        <f aca="false">IF(C68&lt;=20,"Very Low",IF(C68&lt;=36,"Low",IF(C68&lt;=46,"A Little Low",IF(C68&lt;=53,"Average",IF(C68&lt;=63,"A Little High",IF(C68&lt;=80,"High","Very High"))))))</f>
         <v>Very Low</v>
       </c>
     </row>
@@ -2766,4 +2770,33 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>